<commit_message>
system test after adding send Email
</commit_message>
<xml_diff>
--- a/Utilities/Data.xlsx
+++ b/Utilities/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="LoginValid" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sub" sheetId="11" r:id="rId10"/>
     <sheet name="flash" sheetId="12" r:id="rId11"/>
     <sheet name="Coupon" sheetId="13" r:id="rId12"/>
+    <sheet name="SendEmail" sheetId="14" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Clothes!$A$1:$G$51</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="110">
   <si>
     <t>Username</t>
   </si>
@@ -378,6 +379,37 @@
   </si>
   <si>
     <t>code2</t>
+  </si>
+  <si>
+    <t>SenderName</t>
+  </si>
+  <si>
+    <t>senderEmail</t>
+  </si>
+  <si>
+    <t>RecName</t>
+  </si>
+  <si>
+    <t>RecEmails</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Chris@integrant.com'</t>
+  </si>
+  <si>
+    <t>Jihad</t>
+  </si>
+  <si>
+    <t>jMohamed@integrant.com'</t>
+  </si>
+  <si>
+    <t>Hello
+Hope Every thing is Ok</t>
   </si>
 </sst>
 </file>
@@ -487,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -518,6 +550,9 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -841,26 +876,26 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -868,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -876,7 +911,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
     </row>
   </sheetData>
@@ -893,12 +928,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -909,7 +944,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -933,13 +968,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -950,7 +985,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>50</v>
       </c>
@@ -971,16 +1006,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -991,7 +1026,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1005,6 +1040,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E7:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1016,9 +1111,9 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>84</v>
       </c>
@@ -1047,9 +1142,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1057,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>85</v>
       </c>
@@ -1078,9 +1173,9 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>88</v>
       </c>
@@ -1106,9 +1201,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1140,13 +1235,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
     </row>
-    <row r="19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -1163,26 +1258,26 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1229,7 +1324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1276,10 +1371,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
     </row>
   </sheetData>
@@ -1299,15 +1394,15 @@
       <selection activeCell="F2" sqref="F2:F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="11.140625" style="4"/>
-    <col min="6" max="6" width="55.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="59.140625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="11.140625" style="4"/>
+    <col min="1" max="5" width="11.109375" style="4"/>
+    <col min="6" max="6" width="55.44140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="59.109375" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="11.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -1330,7 +1425,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1353,7 +1448,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1376,7 +1471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1399,7 +1494,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1422,7 +1517,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1445,7 +1540,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1468,7 +1563,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1491,7 +1586,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1514,7 +1609,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1537,7 +1632,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1560,7 +1655,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1583,7 +1678,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1606,7 +1701,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1629,7 +1724,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1652,7 +1747,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1675,7 +1770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1698,7 +1793,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1721,7 +1816,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1744,7 +1839,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1767,7 +1862,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1790,7 +1885,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1813,7 +1908,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1836,7 +1931,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1859,7 +1954,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1882,7 +1977,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1905,7 +2000,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1928,7 +2023,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1951,7 +2046,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1974,7 +2069,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1997,7 +2092,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -2020,7 +2115,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -2043,7 +2138,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -2066,7 +2161,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -2089,7 +2184,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -2112,7 +2207,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -2135,7 +2230,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -2158,7 +2253,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -2181,7 +2276,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -2204,7 +2299,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -2227,7 +2322,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -2250,7 +2345,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -2273,7 +2368,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -2296,7 +2391,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -2319,7 +2414,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -2342,7 +2437,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -2365,7 +2460,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -2388,7 +2483,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -2411,7 +2506,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -2434,7 +2529,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -2457,7 +2552,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -2480,7 +2575,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -2489,7 +2584,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -2498,7 +2593,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2507,7 +2602,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2516,7 +2611,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -2525,7 +2620,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -2534,7 +2629,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2543,7 +2638,7 @@
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2552,7 +2647,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2561,7 +2656,7 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2570,7 +2665,7 @@
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -2579,7 +2674,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2588,7 +2683,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -2597,7 +2692,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -2606,7 +2701,7 @@
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -2615,7 +2710,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -2624,7 +2719,7 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -2633,7 +2728,7 @@
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -2642,7 +2737,7 @@
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -2651,7 +2746,7 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -2660,7 +2755,7 @@
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -2669,7 +2764,7 @@
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
@@ -2678,7 +2773,7 @@
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -2687,7 +2782,7 @@
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
@@ -2696,7 +2791,7 @@
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -2705,7 +2800,7 @@
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
@@ -2714,7 +2809,7 @@
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
@@ -2723,7 +2818,7 @@
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -2732,7 +2827,7 @@
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -2741,7 +2836,7 @@
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -2750,7 +2845,7 @@
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -2759,7 +2854,7 @@
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -2768,7 +2863,7 @@
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -2777,7 +2872,7 @@
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -2786,7 +2881,7 @@
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -2795,7 +2890,7 @@
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -2804,7 +2899,7 @@
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -2813,7 +2908,7 @@
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -2822,7 +2917,7 @@
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -2831,7 +2926,7 @@
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -2840,7 +2935,7 @@
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -2849,7 +2944,7 @@
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -2858,7 +2953,7 @@
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -2867,7 +2962,7 @@
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
@@ -2876,7 +2971,7 @@
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
@@ -2885,7 +2980,7 @@
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
@@ -2894,7 +2989,7 @@
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
@@ -2903,7 +2998,7 @@
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
@@ -2912,7 +3007,7 @@
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
@@ -2921,7 +3016,7 @@
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
@@ -2930,7 +3025,7 @@
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -2939,7 +3034,7 @@
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
@@ -2948,7 +3043,7 @@
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
@@ -2957,7 +3052,7 @@
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
@@ -2966,7 +3061,7 @@
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
@@ -2975,7 +3070,7 @@
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
@@ -2984,7 +3079,7 @@
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
@@ -2993,7 +3088,7 @@
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
@@ -3002,7 +3097,7 @@
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
@@ -3011,7 +3106,7 @@
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
@@ -3020,7 +3115,7 @@
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
@@ -3029,7 +3124,7 @@
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
@@ -3038,7 +3133,7 @@
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
@@ -3047,7 +3142,7 @@
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
@@ -3056,7 +3151,7 @@
       <c r="F115" s="5"/>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
@@ -3065,7 +3160,7 @@
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
@@ -3074,7 +3169,7 @@
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
@@ -3083,7 +3178,7 @@
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
@@ -3092,7 +3187,7 @@
       <c r="F119" s="5"/>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
@@ -3101,7 +3196,7 @@
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
@@ -3110,7 +3205,7 @@
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
@@ -3119,7 +3214,7 @@
       <c r="F122" s="5"/>
       <c r="G122" s="5"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
@@ -3128,7 +3223,7 @@
       <c r="F123" s="5"/>
       <c r="G123" s="5"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
@@ -3137,7 +3232,7 @@
       <c r="F124" s="5"/>
       <c r="G124" s="5"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
@@ -3146,7 +3241,7 @@
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
@@ -3155,7 +3250,7 @@
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
@@ -3164,7 +3259,7 @@
       <c r="F127" s="5"/>
       <c r="G127" s="5"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
@@ -3173,7 +3268,7 @@
       <c r="F128" s="5"/>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
@@ -3182,7 +3277,7 @@
       <c r="F129" s="5"/>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
@@ -3191,7 +3286,7 @@
       <c r="F130" s="5"/>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
@@ -3200,7 +3295,7 @@
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
@@ -3209,7 +3304,7 @@
       <c r="F132" s="5"/>
       <c r="G132" s="5"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
@@ -3218,7 +3313,7 @@
       <c r="F133" s="5"/>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
@@ -3227,7 +3322,7 @@
       <c r="F134" s="5"/>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
@@ -3236,7 +3331,7 @@
       <c r="F135" s="5"/>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
@@ -3245,7 +3340,7 @@
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
@@ -3254,7 +3349,7 @@
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
@@ -3263,7 +3358,7 @@
       <c r="F138" s="5"/>
       <c r="G138" s="5"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
@@ -3272,7 +3367,7 @@
       <c r="F139" s="5"/>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
@@ -3281,7 +3376,7 @@
       <c r="F140" s="5"/>
       <c r="G140" s="5"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
@@ -3290,7 +3385,7 @@
       <c r="F141" s="5"/>
       <c r="G141" s="5"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
@@ -3299,7 +3394,7 @@
       <c r="F142" s="5"/>
       <c r="G142" s="5"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
@@ -3308,7 +3403,7 @@
       <c r="F143" s="5"/>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
@@ -3317,7 +3412,7 @@
       <c r="F144" s="5"/>
       <c r="G144" s="5"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
@@ -3326,7 +3421,7 @@
       <c r="F145" s="5"/>
       <c r="G145" s="5"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="5"/>
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
@@ -3335,7 +3430,7 @@
       <c r="F146" s="5"/>
       <c r="G146" s="5"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="5"/>
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
@@ -3344,7 +3439,7 @@
       <c r="F147" s="5"/>
       <c r="G147" s="5"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="5"/>
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
@@ -3353,7 +3448,7 @@
       <c r="F148" s="5"/>
       <c r="G148" s="5"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="5"/>
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
@@ -3362,7 +3457,7 @@
       <c r="F149" s="5"/>
       <c r="G149" s="5"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="5"/>
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
@@ -3371,7 +3466,7 @@
       <c r="F150" s="5"/>
       <c r="G150" s="5"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="5"/>
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
@@ -3380,7 +3475,7 @@
       <c r="F151" s="5"/>
       <c r="G151" s="5"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="5"/>
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
@@ -3389,7 +3484,7 @@
       <c r="F152" s="5"/>
       <c r="G152" s="5"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="5"/>
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
@@ -3398,7 +3493,7 @@
       <c r="F153" s="5"/>
       <c r="G153" s="5"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="5"/>
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
@@ -3407,7 +3502,7 @@
       <c r="F154" s="5"/>
       <c r="G154" s="5"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="5"/>
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
@@ -3416,7 +3511,7 @@
       <c r="F155" s="5"/>
       <c r="G155" s="5"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="5"/>
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
@@ -3425,7 +3520,7 @@
       <c r="F156" s="5"/>
       <c r="G156" s="5"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="5"/>
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
@@ -3434,7 +3529,7 @@
       <c r="F157" s="5"/>
       <c r="G157" s="5"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="5"/>
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
@@ -3443,7 +3538,7 @@
       <c r="F158" s="5"/>
       <c r="G158" s="5"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="5"/>
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
@@ -3452,7 +3547,7 @@
       <c r="F159" s="5"/>
       <c r="G159" s="5"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="5"/>
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
@@ -3461,7 +3556,7 @@
       <c r="F160" s="5"/>
       <c r="G160" s="5"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="5"/>
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
@@ -3470,7 +3565,7 @@
       <c r="F161" s="5"/>
       <c r="G161" s="5"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="5"/>
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
@@ -3479,7 +3574,7 @@
       <c r="F162" s="5"/>
       <c r="G162" s="5"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="5"/>
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
@@ -3488,7 +3583,7 @@
       <c r="F163" s="5"/>
       <c r="G163" s="5"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="5"/>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
@@ -3497,7 +3592,7 @@
       <c r="F164" s="5"/>
       <c r="G164" s="5"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="5"/>
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
@@ -3506,7 +3601,7 @@
       <c r="F165" s="5"/>
       <c r="G165" s="5"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="5"/>
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
@@ -3515,7 +3610,7 @@
       <c r="F166" s="5"/>
       <c r="G166" s="5"/>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="5"/>
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
@@ -3524,7 +3619,7 @@
       <c r="F167" s="5"/>
       <c r="G167" s="5"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="5"/>
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
@@ -3533,7 +3628,7 @@
       <c r="F168" s="5"/>
       <c r="G168" s="5"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="5"/>
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
@@ -3542,7 +3637,7 @@
       <c r="F169" s="5"/>
       <c r="G169" s="5"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="5"/>
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
@@ -3551,7 +3646,7 @@
       <c r="F170" s="5"/>
       <c r="G170" s="5"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
@@ -3560,7 +3655,7 @@
       <c r="F171" s="5"/>
       <c r="G171" s="5"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="5"/>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
@@ -3569,7 +3664,7 @@
       <c r="F172" s="5"/>
       <c r="G172" s="5"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="5"/>
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
@@ -3578,7 +3673,7 @@
       <c r="F173" s="5"/>
       <c r="G173" s="5"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
@@ -3587,7 +3682,7 @@
       <c r="F174" s="5"/>
       <c r="G174" s="5"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="5"/>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
@@ -3596,7 +3691,7 @@
       <c r="F175" s="5"/>
       <c r="G175" s="5"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="5"/>
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
@@ -3605,7 +3700,7 @@
       <c r="F176" s="5"/>
       <c r="G176" s="5"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="5"/>
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
@@ -3614,7 +3709,7 @@
       <c r="F177" s="5"/>
       <c r="G177" s="5"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" s="5"/>
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
@@ -3623,7 +3718,7 @@
       <c r="F178" s="5"/>
       <c r="G178" s="5"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" s="5"/>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
@@ -3632,7 +3727,7 @@
       <c r="F179" s="5"/>
       <c r="G179" s="5"/>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" s="5"/>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
@@ -3641,7 +3736,7 @@
       <c r="F180" s="5"/>
       <c r="G180" s="5"/>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="5"/>
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
@@ -3650,7 +3745,7 @@
       <c r="F181" s="5"/>
       <c r="G181" s="5"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" s="5"/>
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
@@ -3659,7 +3754,7 @@
       <c r="F182" s="5"/>
       <c r="G182" s="5"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" s="5"/>
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
@@ -3668,7 +3763,7 @@
       <c r="F183" s="5"/>
       <c r="G183" s="5"/>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" s="5"/>
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
@@ -3677,7 +3772,7 @@
       <c r="F184" s="5"/>
       <c r="G184" s="5"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" s="5"/>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
@@ -3686,7 +3781,7 @@
       <c r="F185" s="5"/>
       <c r="G185" s="5"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" s="5"/>
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
@@ -3695,7 +3790,7 @@
       <c r="F186" s="5"/>
       <c r="G186" s="5"/>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187" s="5"/>
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
@@ -3704,7 +3799,7 @@
       <c r="F187" s="5"/>
       <c r="G187" s="5"/>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188" s="5"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
@@ -3713,7 +3808,7 @@
       <c r="F188" s="5"/>
       <c r="G188" s="5"/>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" s="5"/>
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
@@ -3722,7 +3817,7 @@
       <c r="F189" s="5"/>
       <c r="G189" s="5"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" s="5"/>
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
@@ -3731,7 +3826,7 @@
       <c r="F190" s="5"/>
       <c r="G190" s="5"/>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" s="5"/>
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
@@ -3740,7 +3835,7 @@
       <c r="F191" s="5"/>
       <c r="G191" s="5"/>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" s="5"/>
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
@@ -3749,7 +3844,7 @@
       <c r="F192" s="5"/>
       <c r="G192" s="5"/>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" s="5"/>
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
@@ -3758,7 +3853,7 @@
       <c r="F193" s="5"/>
       <c r="G193" s="5"/>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" s="5"/>
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
@@ -3767,7 +3862,7 @@
       <c r="F194" s="5"/>
       <c r="G194" s="5"/>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" s="5"/>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -3776,7 +3871,7 @@
       <c r="F195" s="5"/>
       <c r="G195" s="5"/>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" s="5"/>
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
@@ -3785,7 +3880,7 @@
       <c r="F196" s="5"/>
       <c r="G196" s="5"/>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" s="5"/>
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
@@ -3794,7 +3889,7 @@
       <c r="F197" s="5"/>
       <c r="G197" s="5"/>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" s="5"/>
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
@@ -3803,7 +3898,7 @@
       <c r="F198" s="5"/>
       <c r="G198" s="5"/>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" s="5"/>
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
@@ -3812,7 +3907,7 @@
       <c r="F199" s="5"/>
       <c r="G199" s="5"/>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" s="5"/>
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
@@ -3821,7 +3916,7 @@
       <c r="F200" s="5"/>
       <c r="G200" s="5"/>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201" s="5"/>
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
@@ -3830,7 +3925,7 @@
       <c r="F201" s="5"/>
       <c r="G201" s="5"/>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202" s="5"/>
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
@@ -3839,7 +3934,7 @@
       <c r="F202" s="5"/>
       <c r="G202" s="5"/>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203" s="5"/>
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
@@ -3848,7 +3943,7 @@
       <c r="F203" s="5"/>
       <c r="G203" s="5"/>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204" s="5"/>
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
@@ -3857,7 +3952,7 @@
       <c r="F204" s="5"/>
       <c r="G204" s="5"/>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205" s="5"/>
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
@@ -3866,7 +3961,7 @@
       <c r="F205" s="5"/>
       <c r="G205" s="5"/>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206" s="5"/>
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
@@ -3875,7 +3970,7 @@
       <c r="F206" s="5"/>
       <c r="G206" s="5"/>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207" s="5"/>
       <c r="B207" s="5"/>
       <c r="C207" s="5"/>
@@ -3884,7 +3979,7 @@
       <c r="F207" s="5"/>
       <c r="G207" s="5"/>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208" s="5"/>
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
@@ -3893,7 +3988,7 @@
       <c r="F208" s="5"/>
       <c r="G208" s="5"/>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" s="5"/>
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
@@ -3902,7 +3997,7 @@
       <c r="F209" s="5"/>
       <c r="G209" s="5"/>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" s="5"/>
       <c r="B210" s="5"/>
       <c r="C210" s="5"/>
@@ -3911,7 +4006,7 @@
       <c r="F210" s="5"/>
       <c r="G210" s="5"/>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" s="5"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
@@ -3920,7 +4015,7 @@
       <c r="F211" s="5"/>
       <c r="G211" s="5"/>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" s="5"/>
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
@@ -3929,7 +4024,7 @@
       <c r="F212" s="5"/>
       <c r="G212" s="5"/>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="5"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
@@ -3938,7 +4033,7 @@
       <c r="F213" s="5"/>
       <c r="G213" s="5"/>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" s="5"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
@@ -3947,7 +4042,7 @@
       <c r="F214" s="5"/>
       <c r="G214" s="5"/>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215" s="5"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
@@ -3956,7 +4051,7 @@
       <c r="F215" s="5"/>
       <c r="G215" s="5"/>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" s="5"/>
       <c r="B216" s="5"/>
       <c r="C216" s="5"/>
@@ -3965,7 +4060,7 @@
       <c r="F216" s="5"/>
       <c r="G216" s="5"/>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217" s="5"/>
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
@@ -3974,7 +4069,7 @@
       <c r="F217" s="5"/>
       <c r="G217" s="5"/>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" s="5"/>
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
@@ -3983,7 +4078,7 @@
       <c r="F218" s="5"/>
       <c r="G218" s="5"/>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219" s="5"/>
       <c r="B219" s="5"/>
       <c r="C219" s="5"/>
@@ -3992,7 +4087,7 @@
       <c r="F219" s="5"/>
       <c r="G219" s="5"/>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" s="5"/>
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
@@ -4001,7 +4096,7 @@
       <c r="F220" s="5"/>
       <c r="G220" s="5"/>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" s="5"/>
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
@@ -4010,7 +4105,7 @@
       <c r="F221" s="5"/>
       <c r="G221" s="5"/>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" s="5"/>
       <c r="B222" s="5"/>
       <c r="C222" s="5"/>
@@ -4019,7 +4114,7 @@
       <c r="F222" s="5"/>
       <c r="G222" s="5"/>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223" s="5"/>
       <c r="B223" s="5"/>
       <c r="C223" s="5"/>
@@ -4028,7 +4123,7 @@
       <c r="F223" s="5"/>
       <c r="G223" s="5"/>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224" s="5"/>
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
@@ -4037,7 +4132,7 @@
       <c r="F224" s="5"/>
       <c r="G224" s="5"/>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" s="5"/>
       <c r="B225" s="5"/>
       <c r="C225" s="5"/>
@@ -4046,7 +4141,7 @@
       <c r="F225" s="5"/>
       <c r="G225" s="5"/>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" s="5"/>
       <c r="B226" s="5"/>
       <c r="C226" s="5"/>
@@ -4055,7 +4150,7 @@
       <c r="F226" s="5"/>
       <c r="G226" s="5"/>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" s="5"/>
       <c r="B227" s="5"/>
       <c r="C227" s="5"/>
@@ -4064,7 +4159,7 @@
       <c r="F227" s="5"/>
       <c r="G227" s="5"/>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" s="5"/>
       <c r="B228" s="5"/>
       <c r="C228" s="5"/>
@@ -4073,7 +4168,7 @@
       <c r="F228" s="5"/>
       <c r="G228" s="5"/>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" s="5"/>
       <c r="B229" s="5"/>
       <c r="C229" s="5"/>
@@ -4082,7 +4177,7 @@
       <c r="F229" s="5"/>
       <c r="G229" s="5"/>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" s="5"/>
       <c r="B230" s="5"/>
       <c r="C230" s="5"/>
@@ -4091,7 +4186,7 @@
       <c r="F230" s="5"/>
       <c r="G230" s="5"/>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" s="5"/>
       <c r="B231" s="5"/>
       <c r="C231" s="5"/>
@@ -4100,7 +4195,7 @@
       <c r="F231" s="5"/>
       <c r="G231" s="5"/>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" s="5"/>
       <c r="B232" s="5"/>
       <c r="C232" s="5"/>
@@ -4109,7 +4204,7 @@
       <c r="F232" s="5"/>
       <c r="G232" s="5"/>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" s="5"/>
       <c r="B233" s="5"/>
       <c r="C233" s="5"/>
@@ -4118,7 +4213,7 @@
       <c r="F233" s="5"/>
       <c r="G233" s="5"/>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" s="5"/>
       <c r="B234" s="5"/>
       <c r="C234" s="5"/>
@@ -4127,7 +4222,7 @@
       <c r="F234" s="5"/>
       <c r="G234" s="5"/>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" s="5"/>
       <c r="B235" s="5"/>
       <c r="C235" s="5"/>
@@ -4136,7 +4231,7 @@
       <c r="F235" s="5"/>
       <c r="G235" s="5"/>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" s="5"/>
       <c r="B236" s="5"/>
       <c r="C236" s="5"/>
@@ -4145,7 +4240,7 @@
       <c r="F236" s="5"/>
       <c r="G236" s="5"/>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" s="5"/>
       <c r="B237" s="5"/>
       <c r="C237" s="5"/>
@@ -4154,7 +4249,7 @@
       <c r="F237" s="5"/>
       <c r="G237" s="5"/>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" s="5"/>
       <c r="B238" s="5"/>
       <c r="C238" s="5"/>
@@ -4163,7 +4258,7 @@
       <c r="F238" s="5"/>
       <c r="G238" s="5"/>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" s="5"/>
       <c r="B239" s="5"/>
       <c r="C239" s="5"/>
@@ -4172,7 +4267,7 @@
       <c r="F239" s="5"/>
       <c r="G239" s="5"/>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" s="5"/>
       <c r="B240" s="5"/>
       <c r="C240" s="5"/>
@@ -4181,7 +4276,7 @@
       <c r="F240" s="5"/>
       <c r="G240" s="5"/>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241" s="5"/>
       <c r="B241" s="5"/>
       <c r="C241" s="5"/>
@@ -4190,7 +4285,7 @@
       <c r="F241" s="5"/>
       <c r="G241" s="5"/>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242" s="5"/>
       <c r="B242" s="5"/>
       <c r="C242" s="5"/>
@@ -4199,7 +4294,7 @@
       <c r="F242" s="5"/>
       <c r="G242" s="5"/>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243" s="5"/>
       <c r="B243" s="5"/>
       <c r="C243" s="5"/>
@@ -4208,7 +4303,7 @@
       <c r="F243" s="5"/>
       <c r="G243" s="5"/>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244" s="5"/>
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
@@ -4217,7 +4312,7 @@
       <c r="F244" s="5"/>
       <c r="G244" s="5"/>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" s="5"/>
       <c r="B245" s="5"/>
       <c r="C245" s="5"/>
@@ -4226,7 +4321,7 @@
       <c r="F245" s="5"/>
       <c r="G245" s="5"/>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246" s="5"/>
       <c r="B246" s="5"/>
       <c r="C246" s="5"/>
@@ -4235,7 +4330,7 @@
       <c r="F246" s="5"/>
       <c r="G246" s="5"/>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247" s="5"/>
       <c r="B247" s="5"/>
       <c r="C247" s="5"/>
@@ -4244,7 +4339,7 @@
       <c r="F247" s="5"/>
       <c r="G247" s="5"/>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248" s="5"/>
       <c r="B248" s="5"/>
       <c r="C248" s="5"/>
@@ -4253,7 +4348,7 @@
       <c r="F248" s="5"/>
       <c r="G248" s="5"/>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" s="5"/>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
@@ -4262,7 +4357,7 @@
       <c r="F249" s="5"/>
       <c r="G249" s="5"/>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250" s="5"/>
       <c r="B250" s="5"/>
       <c r="C250" s="5"/>
@@ -4271,7 +4366,7 @@
       <c r="F250" s="5"/>
       <c r="G250" s="5"/>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251" s="5"/>
       <c r="B251" s="5"/>
       <c r="C251" s="5"/>
@@ -4280,7 +4375,7 @@
       <c r="F251" s="5"/>
       <c r="G251" s="5"/>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252" s="5"/>
       <c r="B252" s="5"/>
       <c r="C252" s="5"/>
@@ -4289,7 +4384,7 @@
       <c r="F252" s="5"/>
       <c r="G252" s="5"/>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253" s="5"/>
       <c r="B253" s="5"/>
       <c r="C253" s="5"/>
@@ -4298,7 +4393,7 @@
       <c r="F253" s="5"/>
       <c r="G253" s="5"/>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254" s="5"/>
       <c r="B254" s="5"/>
       <c r="C254" s="5"/>
@@ -4307,7 +4402,7 @@
       <c r="F254" s="5"/>
       <c r="G254" s="5"/>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255" s="5"/>
       <c r="B255" s="5"/>
       <c r="C255" s="5"/>
@@ -4316,7 +4411,7 @@
       <c r="F255" s="5"/>
       <c r="G255" s="5"/>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256" s="5"/>
       <c r="B256" s="5"/>
       <c r="C256" s="5"/>
@@ -4325,7 +4420,7 @@
       <c r="F256" s="5"/>
       <c r="G256" s="5"/>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257" s="5"/>
       <c r="B257" s="5"/>
       <c r="C257" s="5"/>
@@ -4334,7 +4429,7 @@
       <c r="F257" s="5"/>
       <c r="G257" s="5"/>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258" s="5"/>
       <c r="B258" s="5"/>
       <c r="C258" s="5"/>
@@ -4343,7 +4438,7 @@
       <c r="F258" s="5"/>
       <c r="G258" s="5"/>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259" s="5"/>
       <c r="B259" s="5"/>
       <c r="C259" s="5"/>
@@ -4352,7 +4447,7 @@
       <c r="F259" s="5"/>
       <c r="G259" s="5"/>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260" s="5"/>
       <c r="B260" s="5"/>
       <c r="C260" s="5"/>
@@ -4361,7 +4456,7 @@
       <c r="F260" s="5"/>
       <c r="G260" s="5"/>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261" s="5"/>
       <c r="B261" s="5"/>
       <c r="C261" s="5"/>
@@ -4370,7 +4465,7 @@
       <c r="F261" s="5"/>
       <c r="G261" s="5"/>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262" s="5"/>
       <c r="B262" s="5"/>
       <c r="C262" s="5"/>
@@ -4379,7 +4474,7 @@
       <c r="F262" s="5"/>
       <c r="G262" s="5"/>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" s="5"/>
       <c r="B263" s="5"/>
       <c r="C263" s="5"/>
@@ -4388,7 +4483,7 @@
       <c r="F263" s="5"/>
       <c r="G263" s="5"/>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264" s="5"/>
       <c r="B264" s="5"/>
       <c r="C264" s="5"/>
@@ -4397,7 +4492,7 @@
       <c r="F264" s="5"/>
       <c r="G264" s="5"/>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265" s="5"/>
       <c r="B265" s="5"/>
       <c r="C265" s="5"/>
@@ -4406,7 +4501,7 @@
       <c r="F265" s="5"/>
       <c r="G265" s="5"/>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266" s="5"/>
       <c r="B266" s="5"/>
       <c r="C266" s="5"/>
@@ -4415,7 +4510,7 @@
       <c r="F266" s="5"/>
       <c r="G266" s="5"/>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267" s="5"/>
       <c r="B267" s="5"/>
       <c r="C267" s="5"/>
@@ -4424,7 +4519,7 @@
       <c r="F267" s="5"/>
       <c r="G267" s="5"/>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268" s="5"/>
       <c r="B268" s="5"/>
       <c r="C268" s="5"/>
@@ -4433,7 +4528,7 @@
       <c r="F268" s="5"/>
       <c r="G268" s="5"/>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269" s="5"/>
       <c r="B269" s="5"/>
       <c r="C269" s="5"/>
@@ -4442,7 +4537,7 @@
       <c r="F269" s="5"/>
       <c r="G269" s="5"/>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270" s="5"/>
       <c r="B270" s="5"/>
       <c r="C270" s="5"/>
@@ -4451,7 +4546,7 @@
       <c r="F270" s="5"/>
       <c r="G270" s="5"/>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271" s="5"/>
       <c r="B271" s="5"/>
       <c r="C271" s="5"/>
@@ -4460,7 +4555,7 @@
       <c r="F271" s="5"/>
       <c r="G271" s="5"/>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272" s="5"/>
       <c r="B272" s="5"/>
       <c r="C272" s="5"/>
@@ -4469,7 +4564,7 @@
       <c r="F272" s="5"/>
       <c r="G272" s="5"/>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273" s="5"/>
       <c r="B273" s="5"/>
       <c r="C273" s="5"/>
@@ -4478,7 +4573,7 @@
       <c r="F273" s="5"/>
       <c r="G273" s="5"/>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" s="5"/>
       <c r="B274" s="5"/>
       <c r="C274" s="5"/>
@@ -4487,7 +4582,7 @@
       <c r="F274" s="5"/>
       <c r="G274" s="5"/>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" s="5"/>
       <c r="B275" s="5"/>
       <c r="C275" s="5"/>
@@ -4496,7 +4591,7 @@
       <c r="F275" s="5"/>
       <c r="G275" s="5"/>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" s="5"/>
       <c r="B276" s="5"/>
       <c r="C276" s="5"/>
@@ -4505,7 +4600,7 @@
       <c r="F276" s="5"/>
       <c r="G276" s="5"/>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" s="5"/>
       <c r="B277" s="5"/>
       <c r="C277" s="5"/>
@@ -4514,7 +4609,7 @@
       <c r="F277" s="5"/>
       <c r="G277" s="5"/>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" s="5"/>
       <c r="B278" s="5"/>
       <c r="C278" s="5"/>
@@ -4523,7 +4618,7 @@
       <c r="F278" s="5"/>
       <c r="G278" s="5"/>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" s="5"/>
       <c r="B279" s="5"/>
       <c r="C279" s="5"/>
@@ -4532,7 +4627,7 @@
       <c r="F279" s="5"/>
       <c r="G279" s="5"/>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280" s="5"/>
       <c r="B280" s="5"/>
       <c r="C280" s="5"/>
@@ -4541,7 +4636,7 @@
       <c r="F280" s="5"/>
       <c r="G280" s="5"/>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" s="5"/>
       <c r="B281" s="5"/>
       <c r="C281" s="5"/>
@@ -4550,7 +4645,7 @@
       <c r="F281" s="5"/>
       <c r="G281" s="5"/>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" s="5"/>
       <c r="B282" s="5"/>
       <c r="C282" s="5"/>
@@ -4559,7 +4654,7 @@
       <c r="F282" s="5"/>
       <c r="G282" s="5"/>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283" s="5"/>
       <c r="B283" s="5"/>
       <c r="C283" s="5"/>
@@ -4568,7 +4663,7 @@
       <c r="F283" s="5"/>
       <c r="G283" s="5"/>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284" s="5"/>
       <c r="B284" s="5"/>
       <c r="C284" s="5"/>
@@ -4577,7 +4672,7 @@
       <c r="F284" s="5"/>
       <c r="G284" s="5"/>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285" s="5"/>
       <c r="B285" s="5"/>
       <c r="C285" s="5"/>
@@ -4586,7 +4681,7 @@
       <c r="F285" s="5"/>
       <c r="G285" s="5"/>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286" s="5"/>
       <c r="B286" s="5"/>
       <c r="C286" s="5"/>
@@ -4595,7 +4690,7 @@
       <c r="F286" s="5"/>
       <c r="G286" s="5"/>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287" s="5"/>
       <c r="B287" s="5"/>
       <c r="C287" s="5"/>
@@ -4604,7 +4699,7 @@
       <c r="F287" s="5"/>
       <c r="G287" s="5"/>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288" s="5"/>
       <c r="B288" s="5"/>
       <c r="C288" s="5"/>
@@ -4613,7 +4708,7 @@
       <c r="F288" s="5"/>
       <c r="G288" s="5"/>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A289" s="5"/>
       <c r="B289" s="5"/>
       <c r="C289" s="5"/>
@@ -4622,7 +4717,7 @@
       <c r="F289" s="5"/>
       <c r="G289" s="5"/>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A290" s="5"/>
       <c r="B290" s="5"/>
       <c r="C290" s="5"/>
@@ -4631,7 +4726,7 @@
       <c r="F290" s="5"/>
       <c r="G290" s="5"/>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A291" s="5"/>
       <c r="B291" s="5"/>
       <c r="C291" s="5"/>
@@ -4640,7 +4735,7 @@
       <c r="F291" s="5"/>
       <c r="G291" s="5"/>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A292" s="5"/>
       <c r="B292" s="5"/>
       <c r="C292" s="5"/>
@@ -4649,7 +4744,7 @@
       <c r="F292" s="5"/>
       <c r="G292" s="5"/>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A293" s="5"/>
       <c r="B293" s="5"/>
       <c r="C293" s="5"/>
@@ -4658,7 +4753,7 @@
       <c r="F293" s="5"/>
       <c r="G293" s="5"/>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A294" s="5"/>
       <c r="B294" s="5"/>
       <c r="C294" s="5"/>
@@ -4667,7 +4762,7 @@
       <c r="F294" s="5"/>
       <c r="G294" s="5"/>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A295" s="5"/>
       <c r="B295" s="5"/>
       <c r="C295" s="5"/>
@@ -4676,7 +4771,7 @@
       <c r="F295" s="5"/>
       <c r="G295" s="5"/>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A296" s="5"/>
       <c r="B296" s="5"/>
       <c r="C296" s="5"/>
@@ -4685,7 +4780,7 @@
       <c r="F296" s="5"/>
       <c r="G296" s="5"/>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A297" s="5"/>
       <c r="B297" s="5"/>
       <c r="C297" s="5"/>
@@ -4694,7 +4789,7 @@
       <c r="F297" s="5"/>
       <c r="G297" s="5"/>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A298" s="5"/>
       <c r="B298" s="5"/>
       <c r="C298" s="5"/>
@@ -4703,7 +4798,7 @@
       <c r="F298" s="5"/>
       <c r="G298" s="5"/>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A299" s="5"/>
       <c r="B299" s="5"/>
       <c r="C299" s="5"/>
@@ -4712,7 +4807,7 @@
       <c r="F299" s="5"/>
       <c r="G299" s="5"/>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A300" s="5"/>
       <c r="B300" s="5"/>
       <c r="C300" s="5"/>
@@ -4721,7 +4816,7 @@
       <c r="F300" s="5"/>
       <c r="G300" s="5"/>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A301" s="5"/>
       <c r="B301" s="5"/>
       <c r="C301" s="5"/>
@@ -4730,7 +4825,7 @@
       <c r="F301" s="5"/>
       <c r="G301" s="5"/>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A302" s="5"/>
       <c r="B302" s="5"/>
       <c r="C302" s="5"/>
@@ -4739,7 +4834,7 @@
       <c r="F302" s="5"/>
       <c r="G302" s="5"/>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A303" s="5"/>
       <c r="B303" s="5"/>
       <c r="C303" s="5"/>
@@ -4748,7 +4843,7 @@
       <c r="F303" s="5"/>
       <c r="G303" s="5"/>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A304" s="5"/>
       <c r="B304" s="5"/>
       <c r="C304" s="5"/>
@@ -4757,7 +4852,7 @@
       <c r="F304" s="5"/>
       <c r="G304" s="5"/>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A305" s="5"/>
       <c r="B305" s="5"/>
       <c r="C305" s="5"/>
@@ -4766,7 +4861,7 @@
       <c r="F305" s="5"/>
       <c r="G305" s="5"/>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A306" s="5"/>
       <c r="B306" s="5"/>
       <c r="C306" s="5"/>
@@ -4775,7 +4870,7 @@
       <c r="F306" s="5"/>
       <c r="G306" s="5"/>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A307" s="5"/>
       <c r="B307" s="5"/>
       <c r="C307" s="5"/>
@@ -4784,7 +4879,7 @@
       <c r="F307" s="5"/>
       <c r="G307" s="5"/>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A308" s="5"/>
       <c r="B308" s="5"/>
       <c r="C308" s="5"/>
@@ -4793,7 +4888,7 @@
       <c r="F308" s="5"/>
       <c r="G308" s="5"/>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A309" s="5"/>
       <c r="B309" s="5"/>
       <c r="C309" s="5"/>
@@ -4802,7 +4897,7 @@
       <c r="F309" s="5"/>
       <c r="G309" s="5"/>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A310" s="5"/>
       <c r="B310" s="5"/>
       <c r="C310" s="5"/>
@@ -4811,7 +4906,7 @@
       <c r="F310" s="5"/>
       <c r="G310" s="5"/>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A311" s="5"/>
       <c r="B311" s="5"/>
       <c r="C311" s="5"/>
@@ -4820,7 +4915,7 @@
       <c r="F311" s="5"/>
       <c r="G311" s="5"/>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A312" s="5"/>
       <c r="B312" s="5"/>
       <c r="C312" s="5"/>
@@ -4829,7 +4924,7 @@
       <c r="F312" s="5"/>
       <c r="G312" s="5"/>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A313" s="5"/>
       <c r="B313" s="5"/>
       <c r="C313" s="5"/>
@@ -4838,7 +4933,7 @@
       <c r="F313" s="5"/>
       <c r="G313" s="5"/>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A314" s="5"/>
       <c r="B314" s="5"/>
       <c r="C314" s="5"/>
@@ -4847,7 +4942,7 @@
       <c r="F314" s="5"/>
       <c r="G314" s="5"/>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A315" s="5"/>
       <c r="B315" s="5"/>
       <c r="C315" s="5"/>
@@ -4856,7 +4951,7 @@
       <c r="F315" s="5"/>
       <c r="G315" s="5"/>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A316" s="5"/>
       <c r="B316" s="5"/>
       <c r="C316" s="5"/>
@@ -4865,7 +4960,7 @@
       <c r="F316" s="5"/>
       <c r="G316" s="5"/>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A317" s="5"/>
       <c r="B317" s="5"/>
       <c r="C317" s="5"/>
@@ -4874,7 +4969,7 @@
       <c r="F317" s="5"/>
       <c r="G317" s="5"/>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A318" s="5"/>
       <c r="B318" s="5"/>
       <c r="C318" s="5"/>
@@ -4883,7 +4978,7 @@
       <c r="F318" s="5"/>
       <c r="G318" s="5"/>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A319" s="5"/>
       <c r="B319" s="5"/>
       <c r="C319" s="5"/>
@@ -4892,7 +4987,7 @@
       <c r="F319" s="5"/>
       <c r="G319" s="5"/>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A320" s="5"/>
       <c r="B320" s="5"/>
       <c r="C320" s="5"/>
@@ -4901,7 +4996,7 @@
       <c r="F320" s="5"/>
       <c r="G320" s="5"/>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A321" s="5"/>
       <c r="B321" s="5"/>
       <c r="C321" s="5"/>
@@ -4910,7 +5005,7 @@
       <c r="F321" s="5"/>
       <c r="G321" s="5"/>
     </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A322" s="5"/>
       <c r="B322" s="5"/>
       <c r="C322" s="5"/>
@@ -4919,7 +5014,7 @@
       <c r="F322" s="5"/>
       <c r="G322" s="5"/>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A323" s="5"/>
       <c r="B323" s="5"/>
       <c r="C323" s="5"/>
@@ -4928,7 +5023,7 @@
       <c r="F323" s="5"/>
       <c r="G323" s="5"/>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A324" s="5"/>
       <c r="B324" s="5"/>
       <c r="C324" s="5"/>
@@ -4937,7 +5032,7 @@
       <c r="F324" s="5"/>
       <c r="G324" s="5"/>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A325" s="5"/>
       <c r="B325" s="5"/>
       <c r="C325" s="5"/>
@@ -4946,7 +5041,7 @@
       <c r="F325" s="5"/>
       <c r="G325" s="5"/>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A326" s="5"/>
       <c r="B326" s="5"/>
       <c r="C326" s="5"/>
@@ -4955,7 +5050,7 @@
       <c r="F326" s="5"/>
       <c r="G326" s="5"/>
     </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A327" s="5"/>
       <c r="B327" s="5"/>
       <c r="C327" s="5"/>
@@ -4964,7 +5059,7 @@
       <c r="F327" s="5"/>
       <c r="G327" s="5"/>
     </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A328" s="5"/>
       <c r="B328" s="5"/>
       <c r="C328" s="5"/>
@@ -4973,7 +5068,7 @@
       <c r="F328" s="5"/>
       <c r="G328" s="5"/>
     </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A329" s="5"/>
       <c r="B329" s="5"/>
       <c r="C329" s="5"/>
@@ -4982,7 +5077,7 @@
       <c r="F329" s="5"/>
       <c r="G329" s="5"/>
     </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A330" s="5"/>
       <c r="B330" s="5"/>
       <c r="C330" s="5"/>
@@ -4991,7 +5086,7 @@
       <c r="F330" s="5"/>
       <c r="G330" s="5"/>
     </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A331" s="5"/>
       <c r="B331" s="5"/>
       <c r="C331" s="5"/>
@@ -5000,7 +5095,7 @@
       <c r="F331" s="5"/>
       <c r="G331" s="5"/>
     </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A332" s="5"/>
       <c r="B332" s="5"/>
       <c r="C332" s="5"/>
@@ -5009,7 +5104,7 @@
       <c r="F332" s="5"/>
       <c r="G332" s="5"/>
     </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A333" s="5"/>
       <c r="B333" s="5"/>
       <c r="C333" s="5"/>
@@ -5018,7 +5113,7 @@
       <c r="F333" s="5"/>
       <c r="G333" s="5"/>
     </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A334" s="5"/>
       <c r="B334" s="5"/>
       <c r="C334" s="5"/>
@@ -5027,7 +5122,7 @@
       <c r="F334" s="5"/>
       <c r="G334" s="5"/>
     </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A335" s="5"/>
       <c r="B335" s="5"/>
       <c r="C335" s="5"/>
@@ -5036,7 +5131,7 @@
       <c r="F335" s="5"/>
       <c r="G335" s="5"/>
     </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A336" s="5"/>
       <c r="B336" s="5"/>
       <c r="C336" s="5"/>
@@ -5045,7 +5140,7 @@
       <c r="F336" s="5"/>
       <c r="G336" s="5"/>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A337" s="5"/>
       <c r="B337" s="5"/>
       <c r="C337" s="5"/>
@@ -5054,7 +5149,7 @@
       <c r="F337" s="5"/>
       <c r="G337" s="5"/>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A338" s="5"/>
       <c r="B338" s="5"/>
       <c r="C338" s="5"/>
@@ -5063,7 +5158,7 @@
       <c r="F338" s="5"/>
       <c r="G338" s="5"/>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A339" s="5"/>
       <c r="B339" s="5"/>
       <c r="C339" s="5"/>
@@ -5072,7 +5167,7 @@
       <c r="F339" s="5"/>
       <c r="G339" s="5"/>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A340" s="5"/>
       <c r="B340" s="5"/>
       <c r="C340" s="5"/>
@@ -5081,7 +5176,7 @@
       <c r="F340" s="5"/>
       <c r="G340" s="5"/>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A341" s="5"/>
       <c r="B341" s="5"/>
       <c r="C341" s="5"/>
@@ -5090,7 +5185,7 @@
       <c r="F341" s="5"/>
       <c r="G341" s="5"/>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A342" s="5"/>
       <c r="B342" s="5"/>
       <c r="C342" s="5"/>
@@ -5099,7 +5194,7 @@
       <c r="F342" s="5"/>
       <c r="G342" s="5"/>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A343" s="5"/>
       <c r="B343" s="5"/>
       <c r="C343" s="5"/>
@@ -5108,7 +5203,7 @@
       <c r="F343" s="5"/>
       <c r="G343" s="5"/>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A344" s="5"/>
       <c r="B344" s="5"/>
       <c r="C344" s="5"/>
@@ -5117,7 +5212,7 @@
       <c r="F344" s="5"/>
       <c r="G344" s="5"/>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A345" s="5"/>
       <c r="B345" s="5"/>
       <c r="C345" s="5"/>
@@ -5126,7 +5221,7 @@
       <c r="F345" s="5"/>
       <c r="G345" s="5"/>
     </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A346" s="5"/>
       <c r="B346" s="5"/>
       <c r="C346" s="5"/>
@@ -5135,7 +5230,7 @@
       <c r="F346" s="5"/>
       <c r="G346" s="5"/>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A347" s="5"/>
       <c r="B347" s="5"/>
       <c r="C347" s="5"/>
@@ -5144,7 +5239,7 @@
       <c r="F347" s="5"/>
       <c r="G347" s="5"/>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A348" s="5"/>
       <c r="B348" s="5"/>
       <c r="C348" s="5"/>
@@ -5153,7 +5248,7 @@
       <c r="F348" s="5"/>
       <c r="G348" s="5"/>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A349" s="5"/>
       <c r="B349" s="5"/>
       <c r="C349" s="5"/>
@@ -5162,7 +5257,7 @@
       <c r="F349" s="5"/>
       <c r="G349" s="5"/>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A350" s="5"/>
       <c r="B350" s="5"/>
       <c r="C350" s="5"/>
@@ -5171,7 +5266,7 @@
       <c r="F350" s="5"/>
       <c r="G350" s="5"/>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A351" s="5"/>
       <c r="B351" s="5"/>
       <c r="C351" s="5"/>
@@ -5180,7 +5275,7 @@
       <c r="F351" s="5"/>
       <c r="G351" s="5"/>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A352" s="5"/>
       <c r="B352" s="5"/>
       <c r="C352" s="5"/>
@@ -5189,7 +5284,7 @@
       <c r="F352" s="5"/>
       <c r="G352" s="5"/>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A353" s="5"/>
       <c r="B353" s="5"/>
       <c r="C353" s="5"/>
@@ -5198,7 +5293,7 @@
       <c r="F353" s="5"/>
       <c r="G353" s="5"/>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A354" s="5"/>
       <c r="B354" s="5"/>
       <c r="C354" s="5"/>
@@ -5207,7 +5302,7 @@
       <c r="F354" s="5"/>
       <c r="G354" s="5"/>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A355" s="5"/>
       <c r="B355" s="5"/>
       <c r="C355" s="5"/>
@@ -5216,7 +5311,7 @@
       <c r="F355" s="5"/>
       <c r="G355" s="5"/>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A356" s="5"/>
       <c r="B356" s="5"/>
       <c r="C356" s="5"/>
@@ -5225,7 +5320,7 @@
       <c r="F356" s="5"/>
       <c r="G356" s="5"/>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A357" s="5"/>
       <c r="B357" s="5"/>
       <c r="C357" s="5"/>
@@ -5234,7 +5329,7 @@
       <c r="F357" s="5"/>
       <c r="G357" s="5"/>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A358" s="5"/>
       <c r="B358" s="5"/>
       <c r="C358" s="5"/>
@@ -5243,7 +5338,7 @@
       <c r="F358" s="5"/>
       <c r="G358" s="5"/>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A359" s="5"/>
       <c r="B359" s="5"/>
       <c r="C359" s="5"/>
@@ -5252,7 +5347,7 @@
       <c r="F359" s="5"/>
       <c r="G359" s="5"/>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A360" s="5"/>
       <c r="B360" s="5"/>
       <c r="C360" s="5"/>
@@ -5261,7 +5356,7 @@
       <c r="F360" s="5"/>
       <c r="G360" s="5"/>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A361" s="5"/>
       <c r="B361" s="5"/>
       <c r="C361" s="5"/>
@@ -5270,7 +5365,7 @@
       <c r="F361" s="5"/>
       <c r="G361" s="5"/>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A362" s="5"/>
       <c r="B362" s="5"/>
       <c r="C362" s="5"/>
@@ -5279,7 +5374,7 @@
       <c r="F362" s="5"/>
       <c r="G362" s="5"/>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A363" s="5"/>
       <c r="B363" s="5"/>
       <c r="C363" s="5"/>
@@ -5288,7 +5383,7 @@
       <c r="F363" s="5"/>
       <c r="G363" s="5"/>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A364" s="5"/>
       <c r="B364" s="5"/>
       <c r="C364" s="5"/>
@@ -5297,7 +5392,7 @@
       <c r="F364" s="5"/>
       <c r="G364" s="5"/>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A365" s="5"/>
       <c r="B365" s="5"/>
       <c r="C365" s="5"/>
@@ -5306,7 +5401,7 @@
       <c r="F365" s="5"/>
       <c r="G365" s="5"/>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A366" s="5"/>
       <c r="B366" s="5"/>
       <c r="C366" s="5"/>
@@ -5315,7 +5410,7 @@
       <c r="F366" s="5"/>
       <c r="G366" s="5"/>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A367" s="5"/>
       <c r="B367" s="5"/>
       <c r="C367" s="5"/>
@@ -5324,7 +5419,7 @@
       <c r="F367" s="5"/>
       <c r="G367" s="5"/>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A368" s="5"/>
       <c r="B368" s="5"/>
       <c r="C368" s="5"/>
@@ -5333,7 +5428,7 @@
       <c r="F368" s="5"/>
       <c r="G368" s="5"/>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A369" s="5"/>
       <c r="B369" s="5"/>
       <c r="C369" s="5"/>
@@ -5342,7 +5437,7 @@
       <c r="F369" s="5"/>
       <c r="G369" s="5"/>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A370" s="5"/>
       <c r="B370" s="5"/>
       <c r="C370" s="5"/>
@@ -5351,7 +5446,7 @@
       <c r="F370" s="5"/>
       <c r="G370" s="5"/>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A371" s="5"/>
       <c r="B371" s="5"/>
       <c r="C371" s="5"/>
@@ -5360,7 +5455,7 @@
       <c r="F371" s="5"/>
       <c r="G371" s="5"/>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A372" s="5"/>
       <c r="B372" s="5"/>
       <c r="C372" s="5"/>
@@ -5369,7 +5464,7 @@
       <c r="F372" s="5"/>
       <c r="G372" s="5"/>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A373" s="5"/>
       <c r="B373" s="5"/>
       <c r="C373" s="5"/>
@@ -5378,7 +5473,7 @@
       <c r="F373" s="5"/>
       <c r="G373" s="5"/>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A374" s="5"/>
       <c r="B374" s="5"/>
       <c r="C374" s="5"/>
@@ -5387,7 +5482,7 @@
       <c r="F374" s="5"/>
       <c r="G374" s="5"/>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A375" s="5"/>
       <c r="B375" s="5"/>
       <c r="C375" s="5"/>
@@ -5396,7 +5491,7 @@
       <c r="F375" s="5"/>
       <c r="G375" s="5"/>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A376" s="5"/>
       <c r="B376" s="5"/>
       <c r="C376" s="5"/>
@@ -5405,7 +5500,7 @@
       <c r="F376" s="5"/>
       <c r="G376" s="5"/>
     </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A377" s="5"/>
       <c r="B377" s="5"/>
       <c r="C377" s="5"/>
@@ -5414,7 +5509,7 @@
       <c r="F377" s="5"/>
       <c r="G377" s="5"/>
     </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A378" s="5"/>
       <c r="B378" s="5"/>
       <c r="C378" s="5"/>
@@ -5423,7 +5518,7 @@
       <c r="F378" s="5"/>
       <c r="G378" s="5"/>
     </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A379" s="5"/>
       <c r="B379" s="5"/>
       <c r="C379" s="5"/>
@@ -5432,7 +5527,7 @@
       <c r="F379" s="5"/>
       <c r="G379" s="5"/>
     </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A380" s="5"/>
       <c r="B380" s="5"/>
       <c r="C380" s="5"/>
@@ -5441,7 +5536,7 @@
       <c r="F380" s="5"/>
       <c r="G380" s="5"/>
     </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A381" s="5"/>
       <c r="B381" s="5"/>
       <c r="C381" s="5"/>
@@ -5467,13 +5562,13 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5487,7 +5582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6</v>
       </c>
@@ -5514,12 +5609,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -5527,7 +5622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Delete Create Address file
</commit_message>
<xml_diff>
--- a/Utilities/Data.xlsx
+++ b/Utilities/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginValid" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
   <si>
     <t>Username</t>
   </si>
@@ -168,9 +168,6 @@
     <t>FR</t>
   </si>
   <si>
-    <t>Thank you</t>
-  </si>
-  <si>
     <t>h0tr1ngG</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
   </si>
   <si>
     <t>Category</t>
-  </si>
-  <si>
-    <t>Clothing</t>
   </si>
   <si>
     <t>trouser</t>
@@ -342,6 +336,9 @@
       </rPr>
       <t>56</t>
     </r>
+  </si>
+  <si>
+    <t>Women</t>
   </si>
 </sst>
 </file>
@@ -855,26 +852,26 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -882,15 +879,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
     </row>
   </sheetData>
@@ -907,47 +904,47 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -965,29 +962,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1003,44 +1000,44 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="72.140625" customWidth="1"/>
+    <col min="5" max="5" width="72.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="D2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1066,14 +1063,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1081,10 +1078,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>42</v>
       </c>
@@ -1092,25 +1089,25 @@
         <v>12</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1129,13 +1126,13 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1149,7 +1146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1170,15 +1167,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J19"/>
+  <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1206,17 +1203,14 @@
       <c r="I2" t="s">
         <v>29</v>
       </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
     </row>
-    <row r="19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -1233,26 +1227,26 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1299,15 +1293,15 @@
         <v>26</v>
       </c>
       <c r="P1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -1349,13 +1343,13 @@
         <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
     </row>
   </sheetData>
@@ -1375,18 +1369,18 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="20"/>
-    <col min="2" max="3" width="11.140625" style="4"/>
-    <col min="4" max="4" width="11.140625" style="20"/>
-    <col min="5" max="5" width="11.140625" style="4"/>
-    <col min="6" max="6" width="55.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="59.140625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="11.140625" style="4"/>
+    <col min="1" max="1" width="11.109375" style="20"/>
+    <col min="2" max="3" width="11.109375" style="4"/>
+    <col min="4" max="4" width="11.109375" style="20"/>
+    <col min="5" max="5" width="11.109375" style="4"/>
+    <col min="6" max="6" width="55.44140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="59.109375" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="11.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>31</v>
       </c>
@@ -1409,7 +1403,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -1423,7 +1417,7 @@
         <v>500</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>39</v>
@@ -1450,30 +1444,30 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1485,42 +1479,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
       <c r="D1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1537,35 +1531,35 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="9.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="16"/>
+    <col min="2" max="3" width="9.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>78</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>80</v>
       </c>
       <c r="D2" s="16">
         <v>300</v>

</xml_diff>